<commit_message>
NM Data from Jun
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
+++ b/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
@@ -31013,19 +31013,19 @@
         </is>
       </c>
       <c r="B2" s="71" t="n">
-        <v>16225759898733.62</v>
+        <v>4658263677133.181</v>
       </c>
       <c r="C2" s="71" t="n">
-        <v>2825023754224.572</v>
+        <v>2401231476316.953</v>
       </c>
       <c r="D2" t="n">
-        <v>3723758241167.105</v>
+        <v>1574550070020.519</v>
       </c>
       <c r="E2" t="n">
-        <v>12114813689698.08</v>
+        <v>4692388216622.726</v>
       </c>
       <c r="F2" t="n">
-        <v>26723939146256.01</v>
+        <v>9387261186199.66</v>
       </c>
       <c r="G2" s="71" t="n">
         <v>1607676980259448</v>
@@ -31039,7 +31039,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>785089739.2296888</v>
+        <v>11346.44320468877</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -31064,16 +31064,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>89405641269870.44</v>
+        <v>22674567101626.41</v>
       </c>
       <c r="C4" t="n">
-        <v>24017229375.92165</v>
+        <v>39957651975.16233</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2532344505600.346</v>
+        <v>1277152099808.283</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -31090,7 +31090,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1309561539526.5</v>
+        <v>107123567930.6255</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -31141,7 +31141,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10529981456924.24</v>
+        <v>1876339772893.282</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -31166,7 +31166,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>61908469304.78194</v>
+        <v>10961252680.95643</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -31216,7 +31216,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>14290619734463.4</v>
+        <v>2274964630162.279</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -31225,7 +31225,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>507413636787.1013</v>
+        <v>236806721023.0075</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -31335,19 +31335,19 @@
         </is>
       </c>
       <c r="B2" s="71" t="n">
-        <v>5910338189579.643</v>
+        <v>1360164846294.702</v>
       </c>
       <c r="C2" s="71" t="n">
-        <v>1029033209246.877</v>
+        <v>701134772154.5624</v>
       </c>
       <c r="D2" t="n">
-        <v>1356403070111.346</v>
+        <v>459752346026.6632</v>
       </c>
       <c r="E2" s="71" t="n">
-        <v>4412899393109.668</v>
+        <v>1370128859117.229</v>
       </c>
       <c r="F2" t="n">
-        <v>9734368010982.748</v>
+        <v>2740983240414.888</v>
       </c>
       <c r="G2">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(About!$A$34,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$80+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(About!$A$34,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$80</f>
@@ -31362,7 +31362,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>285974025.0672946</v>
+        <v>3313.044139870363</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -31387,16 +31387,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>32566584200621.3</v>
+        <v>6620739231224.25</v>
       </c>
       <c r="C4" t="n">
-        <v>8748431437.068325</v>
+        <v>11667221377.76058</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>922422896310.0853</v>
+        <v>372915212605.5195</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -31413,7 +31413,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>477016277017.1563</v>
+        <v>31278974615.40229</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -31464,7 +31464,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3835613982262.991</v>
+        <v>547871819992.0952</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -31489,7 +31489,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22550561124.66137</v>
+        <v>3200572488.237924</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -31539,7 +31539,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5205450844613.547</v>
+        <v>664266158161.0789</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -31548,7 +31548,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>184828705350.8268</v>
+        <v>69145114924.03061</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -31658,19 +31658,19 @@
         </is>
       </c>
       <c r="B2" s="71" t="n">
-        <v>3399873514563.091</v>
+        <v>452734695639.1176</v>
       </c>
       <c r="C2" s="71" t="n">
-        <v>10285779408525.03</v>
+        <v>3827965709408.482</v>
       </c>
       <c r="D2" t="n">
-        <v>8170730457546.817</v>
+        <v>2164341499742.379</v>
       </c>
       <c r="E2" t="n">
-        <v>10723649657837.97</v>
+        <v>3365349370265.354</v>
       </c>
       <c r="F2" t="n">
-        <v>44014821589101.09</v>
+        <v>13784672437536.81</v>
       </c>
       <c r="G2">
         <f>SUM(INDEX('AEO Table 5'!$C$38:$AJ$40,0,MATCH(About!$A$34,'AEO Table 5'!$C$1:$AK$1,0)))*10^15</f>
@@ -31711,19 +31711,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>39226054555061.99</v>
+        <v>7916577724273.482</v>
       </c>
       <c r="C4" t="n">
-        <v>19990326884.72181</v>
+        <v>28385370519.45422</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>8256042633010.897</v>
+        <v>4686150911899.201</v>
       </c>
       <c r="F4" t="n">
-        <v>14614433814665.09</v>
+        <v>4576985109150.229</v>
       </c>
       <c r="G4">
         <f>INDEX('AEO Table 5'!$C$48:$AK$48,MATCH(About!$A$34,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -31737,7 +31737,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2082940787168.423</v>
+        <v>31066702603.90161</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -31746,10 +31746,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>15747402285.40768</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3498601453843.676</v>
+        <v>1095700795539.907</v>
       </c>
       <c r="G5">
         <f>INDEX('AEO Table 5'!$C$54:$AK$54,MATCH(About!$A$34,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -31763,7 +31763,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2528937037967.853</v>
+        <v>710783757265.3558</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>

</xml_diff>